<commit_message>
added vax5.xlsx with analysis for shot 1
</commit_message>
<xml_diff>
--- a/analysis/ChatGPT ASMR.xlsx
+++ b/analysis/ChatGPT ASMR.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\Czech\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDB7F131-73D9-4ECF-9B3D-7C823A164DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2220599-AC9C-4441-A89D-C87C33D7A2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-690" yWindow="945" windowWidth="16110" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Tables with Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="about this data" sheetId="3" r:id="rId2"/>
+    <sheet name="Summary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="51">
   <si>
     <t>age</t>
   </si>
@@ -166,6 +167,27 @@
   </si>
   <si>
     <t>&lt;&lt;&lt;--- very large increase</t>
+  </si>
+  <si>
+    <t>This data was extracted from the vax5, vax6, and vax7 csv files</t>
+  </si>
+  <si>
+    <t>I imported into excel and did pivot tables and copied them over to thei spreadsheet</t>
+  </si>
+  <si>
+    <t>then I added the age standard (US) to compute the ASMR</t>
+  </si>
+  <si>
+    <t>vax 5 gives dose 1 numbers</t>
+  </si>
+  <si>
+    <t>vax 6 gives dose 2 numbesr</t>
+  </si>
+  <si>
+    <t>vax7 gives dose 3 numbesr</t>
+  </si>
+  <si>
+    <t>see anallysis/vax_5.xlsx for the pivot table for dose 1</t>
   </si>
 </sst>
 </file>
@@ -239,10 +261,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1574,12 +1596,12 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -1602,7 +1624,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1623,7 +1645,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -1648,7 +1670,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1673,7 +1695,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -1698,7 +1720,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1723,7 +1745,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1748,7 +1770,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -1773,7 +1795,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -1798,7 +1820,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -1826,7 +1848,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>22</v>
       </c>
@@ -1851,7 +1873,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -1876,7 +1898,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -1901,7 +1923,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>25</v>
       </c>
@@ -1926,7 +1948,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -1951,7 +1973,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>27</v>
       </c>
@@ -1976,7 +1998,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -2001,7 +2023,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>29</v>
       </c>
@@ -2026,7 +2048,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>30</v>
       </c>
@@ -2051,7 +2073,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>31</v>
       </c>
@@ -2076,7 +2098,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -2094,7 +2116,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
@@ -2117,7 +2139,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -2138,7 +2160,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2181,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="4"/>
       <c r="B26" t="s">
         <v>16</v>
       </c>
@@ -2180,7 +2202,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="4"/>
       <c r="B27" t="s">
         <v>17</v>
       </c>
@@ -2201,7 +2223,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="4"/>
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -2222,7 +2244,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="4"/>
       <c r="B29" t="s">
         <v>19</v>
       </c>
@@ -2243,7 +2265,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>21</v>
       </c>
@@ -2264,7 +2286,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>22</v>
       </c>
@@ -2285,7 +2307,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="4"/>
       <c r="B32" t="s">
         <v>23</v>
       </c>
@@ -2306,7 +2328,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="4"/>
       <c r="B33" t="s">
         <v>24</v>
       </c>
@@ -2327,7 +2349,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="A34" s="4"/>
       <c r="B34" t="s">
         <v>25</v>
       </c>
@@ -2348,7 +2370,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="A35" s="4"/>
       <c r="B35" t="s">
         <v>26</v>
       </c>
@@ -2369,7 +2391,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="4"/>
       <c r="B36" t="s">
         <v>27</v>
       </c>
@@ -2390,7 +2412,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="4"/>
       <c r="B37" t="s">
         <v>28</v>
       </c>
@@ -2411,7 +2433,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="4"/>
       <c r="B38" t="s">
         <v>29</v>
       </c>
@@ -2432,7 +2454,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="4"/>
       <c r="B39" t="s">
         <v>30</v>
       </c>
@@ -2453,7 +2475,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="4"/>
       <c r="B40" t="s">
         <v>31</v>
       </c>
@@ -2474,7 +2496,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="4"/>
       <c r="B41" t="s">
         <v>32</v>
       </c>
@@ -2492,7 +2514,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B42" t="s">
@@ -2515,7 +2537,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="4"/>
       <c r="B43" t="s">
         <v>13</v>
       </c>
@@ -2536,7 +2558,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="4"/>
       <c r="B44" t="s">
         <v>14</v>
       </c>
@@ -2557,7 +2579,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="4"/>
       <c r="B45" t="s">
         <v>15</v>
       </c>
@@ -2578,7 +2600,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="4"/>
       <c r="B46" t="s">
         <v>16</v>
       </c>
@@ -2599,7 +2621,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="4"/>
       <c r="B47" t="s">
         <v>17</v>
       </c>
@@ -2620,7 +2642,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
+      <c r="A48" s="4"/>
       <c r="B48" t="s">
         <v>18</v>
       </c>
@@ -2641,7 +2663,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+      <c r="A49" s="4"/>
       <c r="B49" t="s">
         <v>19</v>
       </c>
@@ -2662,7 +2684,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
+      <c r="A50" s="4"/>
       <c r="B50" t="s">
         <v>20</v>
       </c>
@@ -2683,7 +2705,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+      <c r="A51" s="4"/>
       <c r="B51" t="s">
         <v>21</v>
       </c>
@@ -2704,7 +2726,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
+      <c r="A52" s="4"/>
       <c r="B52" t="s">
         <v>22</v>
       </c>
@@ -2725,7 +2747,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
+      <c r="A53" s="4"/>
       <c r="B53" t="s">
         <v>23</v>
       </c>
@@ -2746,7 +2768,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+      <c r="A54" s="4"/>
       <c r="B54" t="s">
         <v>24</v>
       </c>
@@ -2767,7 +2789,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="4"/>
       <c r="B55" t="s">
         <v>25</v>
       </c>
@@ -2788,7 +2810,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
+      <c r="A56" s="4"/>
       <c r="B56" t="s">
         <v>26</v>
       </c>
@@ -2809,7 +2831,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
+      <c r="A57" s="4"/>
       <c r="B57" t="s">
         <v>27</v>
       </c>
@@ -2830,7 +2852,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
+      <c r="A58" s="4"/>
       <c r="B58" t="s">
         <v>28</v>
       </c>
@@ -2851,7 +2873,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
+      <c r="A59" s="4"/>
       <c r="B59" t="s">
         <v>29</v>
       </c>
@@ -2872,7 +2894,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
+      <c r="A60" s="4"/>
       <c r="B60" t="s">
         <v>30</v>
       </c>
@@ -2893,7 +2915,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
+      <c r="A61" s="4"/>
       <c r="B61" t="s">
         <v>31</v>
       </c>
@@ -2914,7 +2936,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
+      <c r="A62" s="4"/>
       <c r="B62" t="s">
         <v>32</v>
       </c>
@@ -2932,7 +2954,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B63" t="s">
@@ -2955,7 +2977,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
+      <c r="A64" s="4"/>
       <c r="B64" t="s">
         <v>14</v>
       </c>
@@ -2976,7 +2998,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
+      <c r="A65" s="4"/>
       <c r="B65" t="s">
         <v>15</v>
       </c>
@@ -2997,7 +3019,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
+      <c r="A66" s="4"/>
       <c r="B66" t="s">
         <v>16</v>
       </c>
@@ -3018,7 +3040,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
+      <c r="A67" s="4"/>
       <c r="B67" t="s">
         <v>17</v>
       </c>
@@ -3039,7 +3061,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
+      <c r="A68" s="4"/>
       <c r="B68" t="s">
         <v>18</v>
       </c>
@@ -3060,7 +3082,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
+      <c r="A69" s="4"/>
       <c r="B69" t="s">
         <v>19</v>
       </c>
@@ -3081,7 +3103,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
+      <c r="A70" s="4"/>
       <c r="B70" t="s">
         <v>21</v>
       </c>
@@ -3102,7 +3124,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
+      <c r="A71" s="4"/>
       <c r="B71" t="s">
         <v>22</v>
       </c>
@@ -3123,7 +3145,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
+      <c r="A72" s="4"/>
       <c r="B72" t="s">
         <v>23</v>
       </c>
@@ -3144,7 +3166,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
+      <c r="A73" s="4"/>
       <c r="B73" t="s">
         <v>24</v>
       </c>
@@ -3165,7 +3187,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
+      <c r="A74" s="4"/>
       <c r="B74" t="s">
         <v>25</v>
       </c>
@@ -3186,7 +3208,7 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
+      <c r="A75" s="4"/>
       <c r="B75" t="s">
         <v>26</v>
       </c>
@@ -3207,7 +3229,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
+      <c r="A76" s="4"/>
       <c r="B76" t="s">
         <v>27</v>
       </c>
@@ -3228,7 +3250,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
+      <c r="A77" s="4"/>
       <c r="B77" t="s">
         <v>28</v>
       </c>
@@ -3249,7 +3271,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
+      <c r="A78" s="4"/>
       <c r="B78" t="s">
         <v>29</v>
       </c>
@@ -3270,7 +3292,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
+      <c r="A79" s="4"/>
       <c r="B79" t="s">
         <v>30</v>
       </c>
@@ -3291,7 +3313,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
+      <c r="A80" s="4"/>
       <c r="B80" t="s">
         <v>31</v>
       </c>
@@ -3312,7 +3334,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
+      <c r="A81" s="4"/>
       <c r="B81" t="s">
         <v>32</v>
       </c>
@@ -3330,7 +3352,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B82" t="s">
@@ -3353,7 +3375,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
+      <c r="A83" s="4"/>
       <c r="B83" t="s">
         <v>14</v>
       </c>
@@ -3374,7 +3396,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
+      <c r="A84" s="4"/>
       <c r="B84" t="s">
         <v>15</v>
       </c>
@@ -3395,7 +3417,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
+      <c r="A85" s="4"/>
       <c r="B85" t="s">
         <v>16</v>
       </c>
@@ -3416,7 +3438,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
+      <c r="A86" s="4"/>
       <c r="B86" t="s">
         <v>17</v>
       </c>
@@ -3437,7 +3459,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
+      <c r="A87" s="4"/>
       <c r="B87" t="s">
         <v>18</v>
       </c>
@@ -3458,7 +3480,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
+      <c r="A88" s="4"/>
       <c r="B88" t="s">
         <v>19</v>
       </c>
@@ -3479,7 +3501,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
+      <c r="A89" s="4"/>
       <c r="B89" t="s">
         <v>21</v>
       </c>
@@ -3500,7 +3522,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
+      <c r="A90" s="4"/>
       <c r="B90" t="s">
         <v>22</v>
       </c>
@@ -3521,7 +3543,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
+      <c r="A91" s="4"/>
       <c r="B91" t="s">
         <v>23</v>
       </c>
@@ -3542,7 +3564,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
+      <c r="A92" s="4"/>
       <c r="B92" t="s">
         <v>24</v>
       </c>
@@ -3563,7 +3585,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
+      <c r="A93" s="4"/>
       <c r="B93" t="s">
         <v>25</v>
       </c>
@@ -3584,7 +3606,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="3"/>
+      <c r="A94" s="4"/>
       <c r="B94" t="s">
         <v>26</v>
       </c>
@@ -3605,7 +3627,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="3"/>
+      <c r="A95" s="4"/>
       <c r="B95" t="s">
         <v>27</v>
       </c>
@@ -3626,7 +3648,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="3"/>
+      <c r="A96" s="4"/>
       <c r="B96" t="s">
         <v>28</v>
       </c>
@@ -3647,7 +3669,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="3"/>
+      <c r="A97" s="4"/>
       <c r="B97" t="s">
         <v>29</v>
       </c>
@@ -3668,7 +3690,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="3"/>
+      <c r="A98" s="4"/>
       <c r="B98" t="s">
         <v>30</v>
       </c>
@@ -3689,7 +3711,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="3"/>
+      <c r="A99" s="4"/>
       <c r="B99" t="s">
         <v>31</v>
       </c>
@@ -3710,7 +3732,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
+      <c r="A100" s="4"/>
       <c r="B100" t="s">
         <v>32</v>
       </c>
@@ -3728,7 +3750,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B101" t="s">
@@ -3751,7 +3773,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="3"/>
+      <c r="A102" s="4"/>
       <c r="B102" t="s">
         <v>14</v>
       </c>
@@ -3772,7 +3794,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="3"/>
+      <c r="A103" s="4"/>
       <c r="B103" t="s">
         <v>15</v>
       </c>
@@ -3793,7 +3815,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="3"/>
+      <c r="A104" s="4"/>
       <c r="B104" t="s">
         <v>16</v>
       </c>
@@ -3814,7 +3836,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
+      <c r="A105" s="4"/>
       <c r="B105" t="s">
         <v>17</v>
       </c>
@@ -3835,7 +3857,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="3"/>
+      <c r="A106" s="4"/>
       <c r="B106" t="s">
         <v>18</v>
       </c>
@@ -3856,7 +3878,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="3"/>
+      <c r="A107" s="4"/>
       <c r="B107" t="s">
         <v>19</v>
       </c>
@@ -3877,7 +3899,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="3"/>
+      <c r="A108" s="4"/>
       <c r="B108" t="s">
         <v>21</v>
       </c>
@@ -3898,7 +3920,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="3"/>
+      <c r="A109" s="4"/>
       <c r="B109" t="s">
         <v>22</v>
       </c>
@@ -3919,7 +3941,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="3"/>
+      <c r="A110" s="4"/>
       <c r="B110" t="s">
         <v>23</v>
       </c>
@@ -3940,7 +3962,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="3"/>
+      <c r="A111" s="4"/>
       <c r="B111" t="s">
         <v>24</v>
       </c>
@@ -3961,7 +3983,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="3"/>
+      <c r="A112" s="4"/>
       <c r="B112" t="s">
         <v>25</v>
       </c>
@@ -3982,7 +4004,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="3"/>
+      <c r="A113" s="4"/>
       <c r="B113" t="s">
         <v>26</v>
       </c>
@@ -4003,7 +4025,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="3"/>
+      <c r="A114" s="4"/>
       <c r="B114" t="s">
         <v>27</v>
       </c>
@@ -4024,7 +4046,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="3"/>
+      <c r="A115" s="4"/>
       <c r="B115" t="s">
         <v>28</v>
       </c>
@@ -4045,7 +4067,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="3"/>
+      <c r="A116" s="4"/>
       <c r="B116" t="s">
         <v>29</v>
       </c>
@@ -4066,7 +4088,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="3"/>
+      <c r="A117" s="4"/>
       <c r="B117" t="s">
         <v>30</v>
       </c>
@@ -4087,7 +4109,7 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
+      <c r="A118" s="4"/>
       <c r="B118" t="s">
         <v>31</v>
       </c>
@@ -4108,7 +4130,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="3"/>
+      <c r="A119" s="4"/>
       <c r="B119" t="s">
         <v>32</v>
       </c>
@@ -4140,6 +4162,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F392971E-973C-4657-A5ED-34AC954671F6}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>

</xml_diff>

<commit_message>
lots of updates including the word doc
</commit_message>
<xml_diff>
--- a/analysis/ChatGPT ASMR.xlsx
+++ b/analysis/ChatGPT ASMR.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\Czech\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2220599-AC9C-4441-A89D-C87C33D7A2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ABE8A7-5270-4C93-A814-5721F6C836D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-690" yWindow="945" windowWidth="16110" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Combined Tables with Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="about this data" sheetId="3" r:id="rId2"/>
-    <sheet name="Summary" sheetId="2" r:id="rId3"/>
+    <sheet name="Summary" sheetId="2" r:id="rId1"/>
+    <sheet name="Combined Tables with Summary" sheetId="1" r:id="rId2"/>
+    <sheet name="about this data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1565,11 +1565,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2">
+        <v>425.09751825406403</v>
+      </c>
+      <c r="C2" s="2">
+        <v>564.08415673002901</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.3269523638877001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.2986017241913601</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.3559219452936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2">
+        <v>418.16429923431701</v>
+      </c>
+      <c r="C3" s="2">
+        <v>548.70093762952399</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.3121659085537101</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.2834354321400101</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.3415395340143199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="2">
+        <v>427.46820274000697</v>
+      </c>
+      <c r="C4" s="2">
+        <v>510.68516448355803</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.1946740394025599</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.1654976074382599</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.22458085826489</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4161,7 +4256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F392971E-973C-4657-A5ED-34AC954671F6}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -4209,99 +4304,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2">
-        <v>425.09751825406403</v>
-      </c>
-      <c r="C2" s="2">
-        <v>564.08415673002901</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.3269523638877001</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.2986017241913601</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.3559219452936</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="2">
-        <v>418.16429923431701</v>
-      </c>
-      <c r="C3" s="2">
-        <v>548.70093762952399</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.3121659085537101</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.2834354321400101</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.3415395340143199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="2">
-        <v>427.46820274000697</v>
-      </c>
-      <c r="C4" s="2">
-        <v>510.68516448355803</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.1946740394025599</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.1654976074382599</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.22458085826489</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>